<commit_message>
Revert "Init Sim Journal"
This reverts commit 8270c62c90a7eec9cfbcde6f8323018642b45105.
</commit_message>
<xml_diff>
--- a/para/Swi/IKQ75N120CS6.xlsx
+++ b/para/Swi/IKQ75N120CS6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f215465b21b5e6e2/Studium/34_Github/PyPowerSim/para/Swi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f215465b21b5e6e2/Studium/02_Herts/03_VRF/23_PE/05_PWM_Losses/para/Swi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1503" documentId="11_AD4DB114E441178AC67DF439BED5CE16693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C20F8F-F0DB-4C42-B59B-A69B0E501BD4}"/>
+  <xr:revisionPtr revIDLastSave="1502" documentId="11_AD4DB114E441178AC67DF439BED5CE16693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD091601-B78A-44AE-BE59-569BC2C80239}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,6 +937,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,15 +953,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -19364,6 +19364,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -19749,7 +19753,7 @@
   <dimension ref="A1:AD184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="A13" sqref="A13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20230,7 +20234,7 @@
         <v>157</v>
       </c>
       <c r="E15" s="16">
-        <v>75</v>
+        <v>600</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -20614,36 +20618,36 @@
     </row>
     <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="45"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="42"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="42"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="45"/>
     </row>
     <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="32"/>
@@ -20882,36 +20886,36 @@
     </row>
     <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="45"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="42"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="42"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="44"/>
+      <c r="K53" s="45"/>
     </row>
     <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="33"/>
@@ -21158,36 +21162,36 @@
     </row>
     <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="44"/>
-      <c r="J72" s="44"/>
-      <c r="K72" s="45"/>
+      <c r="B72" s="41"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="41"/>
+      <c r="K72" s="42"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C73" s="41"/>
-      <c r="D73" s="41"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="41"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="41"/>
-      <c r="I73" s="41"/>
-      <c r="J73" s="41"/>
-      <c r="K73" s="42"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="45"/>
     </row>
     <row r="74" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="34"/>
@@ -21434,36 +21438,36 @@
     </row>
     <row r="91" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="43" t="s">
+      <c r="A92" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B92" s="44"/>
-      <c r="C92" s="44"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="44"/>
-      <c r="I92" s="44"/>
-      <c r="J92" s="44"/>
-      <c r="K92" s="45"/>
+      <c r="B92" s="41"/>
+      <c r="C92" s="41"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="41"/>
+      <c r="F92" s="41"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="41"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="41"/>
+      <c r="K92" s="42"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B93" s="40" t="s">
+      <c r="B93" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C93" s="41"/>
-      <c r="D93" s="41"/>
-      <c r="E93" s="41"/>
-      <c r="F93" s="41"/>
-      <c r="G93" s="41"/>
-      <c r="H93" s="41"/>
-      <c r="I93" s="41"/>
-      <c r="J93" s="41"/>
-      <c r="K93" s="42"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="44"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="44"/>
+      <c r="K93" s="45"/>
     </row>
     <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="32"/>
@@ -21718,37 +21722,37 @@
     </row>
     <row r="111" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A112" s="43" t="s">
+      <c r="A112" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B112" s="44"/>
-      <c r="C112" s="44"/>
-      <c r="D112" s="44"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="44"/>
-      <c r="G112" s="44"/>
-      <c r="H112" s="44"/>
-      <c r="I112" s="44"/>
-      <c r="J112" s="44"/>
-      <c r="K112" s="45"/>
+      <c r="B112" s="41"/>
+      <c r="C112" s="41"/>
+      <c r="D112" s="41"/>
+      <c r="E112" s="41"/>
+      <c r="F112" s="41"/>
+      <c r="G112" s="41"/>
+      <c r="H112" s="41"/>
+      <c r="I112" s="41"/>
+      <c r="J112" s="41"/>
+      <c r="K112" s="42"/>
       <c r="L112" s="2"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C113" s="41"/>
-      <c r="D113" s="41"/>
-      <c r="E113" s="41"/>
-      <c r="F113" s="41"/>
-      <c r="G113" s="41"/>
-      <c r="H113" s="41"/>
-      <c r="I113" s="41"/>
-      <c r="J113" s="41"/>
-      <c r="K113" s="42"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="44"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="44"/>
+      <c r="I113" s="44"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="45"/>
       <c r="L113" s="1"/>
     </row>
     <row r="114" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21999,36 +22003,36 @@
     </row>
     <row r="131" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="132" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A132" s="43" t="s">
+      <c r="A132" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="B132" s="44"/>
-      <c r="C132" s="44"/>
-      <c r="D132" s="44"/>
-      <c r="E132" s="44"/>
-      <c r="F132" s="44"/>
-      <c r="G132" s="44"/>
-      <c r="H132" s="44"/>
-      <c r="I132" s="44"/>
-      <c r="J132" s="44"/>
-      <c r="K132" s="45"/>
+      <c r="B132" s="41"/>
+      <c r="C132" s="41"/>
+      <c r="D132" s="41"/>
+      <c r="E132" s="41"/>
+      <c r="F132" s="41"/>
+      <c r="G132" s="41"/>
+      <c r="H132" s="41"/>
+      <c r="I132" s="41"/>
+      <c r="J132" s="41"/>
+      <c r="K132" s="42"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="B133" s="40" t="s">
+      <c r="B133" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C133" s="41"/>
-      <c r="D133" s="41"/>
-      <c r="E133" s="41"/>
-      <c r="F133" s="41"/>
-      <c r="G133" s="41"/>
-      <c r="H133" s="41"/>
-      <c r="I133" s="41"/>
-      <c r="J133" s="41"/>
-      <c r="K133" s="42"/>
+      <c r="C133" s="44"/>
+      <c r="D133" s="44"/>
+      <c r="E133" s="44"/>
+      <c r="F133" s="44"/>
+      <c r="G133" s="44"/>
+      <c r="H133" s="44"/>
+      <c r="I133" s="44"/>
+      <c r="J133" s="44"/>
+      <c r="K133" s="45"/>
     </row>
     <row r="134" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="32"/>
@@ -22235,36 +22239,36 @@
     </row>
     <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A152" s="43" t="s">
+      <c r="A152" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B152" s="44"/>
-      <c r="C152" s="44"/>
-      <c r="D152" s="44"/>
-      <c r="E152" s="44"/>
-      <c r="F152" s="44"/>
-      <c r="G152" s="44"/>
-      <c r="H152" s="44"/>
-      <c r="I152" s="44"/>
-      <c r="J152" s="44"/>
-      <c r="K152" s="45"/>
+      <c r="B152" s="41"/>
+      <c r="C152" s="41"/>
+      <c r="D152" s="41"/>
+      <c r="E152" s="41"/>
+      <c r="F152" s="41"/>
+      <c r="G152" s="41"/>
+      <c r="H152" s="41"/>
+      <c r="I152" s="41"/>
+      <c r="J152" s="41"/>
+      <c r="K152" s="42"/>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="B153" s="40" t="s">
+      <c r="B153" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C153" s="41"/>
-      <c r="D153" s="41"/>
-      <c r="E153" s="41"/>
-      <c r="F153" s="41"/>
-      <c r="G153" s="41"/>
-      <c r="H153" s="41"/>
-      <c r="I153" s="41"/>
-      <c r="J153" s="41"/>
-      <c r="K153" s="42"/>
+      <c r="C153" s="44"/>
+      <c r="D153" s="44"/>
+      <c r="E153" s="44"/>
+      <c r="F153" s="44"/>
+      <c r="G153" s="44"/>
+      <c r="H153" s="44"/>
+      <c r="I153" s="44"/>
+      <c r="J153" s="44"/>
+      <c r="K153" s="45"/>
     </row>
     <row r="154" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="32"/>
@@ -22471,36 +22475,36 @@
     </row>
     <row r="171" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A172" s="43" t="s">
+      <c r="A172" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="B172" s="44"/>
-      <c r="C172" s="44"/>
-      <c r="D172" s="44"/>
-      <c r="E172" s="44"/>
-      <c r="F172" s="44"/>
-      <c r="G172" s="44"/>
-      <c r="H172" s="44"/>
-      <c r="I172" s="44"/>
-      <c r="J172" s="44"/>
-      <c r="K172" s="45"/>
+      <c r="B172" s="41"/>
+      <c r="C172" s="41"/>
+      <c r="D172" s="41"/>
+      <c r="E172" s="41"/>
+      <c r="F172" s="41"/>
+      <c r="G172" s="41"/>
+      <c r="H172" s="41"/>
+      <c r="I172" s="41"/>
+      <c r="J172" s="41"/>
+      <c r="K172" s="42"/>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="B173" s="40" t="s">
+      <c r="B173" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C173" s="41"/>
-      <c r="D173" s="41"/>
-      <c r="E173" s="41"/>
-      <c r="F173" s="41"/>
-      <c r="G173" s="41"/>
-      <c r="H173" s="41"/>
-      <c r="I173" s="41"/>
-      <c r="J173" s="41"/>
-      <c r="K173" s="42"/>
+      <c r="C173" s="44"/>
+      <c r="D173" s="44"/>
+      <c r="E173" s="44"/>
+      <c r="F173" s="44"/>
+      <c r="G173" s="44"/>
+      <c r="H173" s="44"/>
+      <c r="I173" s="44"/>
+      <c r="J173" s="44"/>
+      <c r="K173" s="45"/>
     </row>
     <row r="174" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="32"/>
@@ -22707,22 +22711,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B73:K73"/>
+    <mergeCell ref="A92:K92"/>
+    <mergeCell ref="B93:K93"/>
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="B113:K113"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="B53:K53"/>
+    <mergeCell ref="A72:K72"/>
     <mergeCell ref="A152:K152"/>
     <mergeCell ref="B153:K153"/>
     <mergeCell ref="A172:K172"/>
     <mergeCell ref="B173:K173"/>
     <mergeCell ref="A132:K132"/>
     <mergeCell ref="B133:K133"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="B53:K53"/>
-    <mergeCell ref="A72:K72"/>
-    <mergeCell ref="B73:K73"/>
-    <mergeCell ref="A92:K92"/>
-    <mergeCell ref="B93:K93"/>
-    <mergeCell ref="A112:K112"/>
-    <mergeCell ref="B113:K113"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>